<commit_message>
update entity, create new logic, controller
</commit_message>
<xml_diff>
--- a/src/main/resources/customers.xlsx
+++ b/src/main/resources/customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Java\MyProject1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB62189-9DC7-4283-B39F-EEF55093204D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D0CD9C-BCE9-4282-842F-E461F3E94DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A31AC8A9-9CDE-4454-8699-485022C98968}"/>
   </bookViews>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -48,9 +39,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>phonenumber</t>
-  </si>
-  <si>
     <t>isAdmin</t>
   </si>
   <si>
@@ -73,6 +61,9 @@
   </si>
   <si>
     <t>03131313131</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
   </si>
 </sst>
 </file>
@@ -432,7 +423,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -455,15 +446,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -472,10 +463,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -483,7 +474,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -492,10 +483,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -503,7 +494,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -512,10 +503,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -523,7 +514,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -532,10 +523,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -543,7 +534,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -552,10 +543,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -563,7 +554,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -572,10 +563,10 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -583,7 +574,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -592,10 +583,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -603,7 +594,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -612,10 +603,10 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -623,7 +614,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -632,10 +623,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -643,7 +634,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -652,10 +643,10 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -663,7 +654,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -672,10 +663,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -683,7 +674,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -692,10 +683,10 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -703,7 +694,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -712,10 +703,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -723,7 +714,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -732,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -743,7 +734,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -752,10 +743,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -763,7 +754,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -772,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -783,7 +774,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -792,10 +783,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -803,7 +794,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -812,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -823,7 +814,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -832,10 +823,10 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>

</xml_diff>